<commit_message>
Servers version and gameplay info
</commit_message>
<xml_diff>
--- a/TSS_boardgame.xlsx
+++ b/TSS_boardgame.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benoi\Desktop\TSS\Thousand-Suns-Saga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81EAD88B-4BEB-4504-8375-DD5FA1F15DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474A3AF3-3195-4CE9-BF95-54DBD270379E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B955C5A0-8230-4033-B161-BBE75800DDCF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B955C5A0-8230-4033-B161-BBE75800DDCF}"/>
   </bookViews>
   <sheets>
     <sheet name="MapGenerator" sheetId="12" r:id="rId1"/>
@@ -10887,8 +10887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F62D196-CE0D-4FC4-B594-4D58D173DB05}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18499,8 +18499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C96B8AE4-0FD4-4126-AACD-9736F4C81F06}">
   <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18624,7 +18624,7 @@
         <v>250</v>
       </c>
       <c r="G5" s="1">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="H5" s="1">
         <v>150</v>
@@ -18653,7 +18653,7 @@
         <v>350</v>
       </c>
       <c r="G6" s="1">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="H6" s="1">
         <v>250</v>
@@ -19169,7 +19169,7 @@
       </c>
       <c r="G36" s="1">
         <f>(G5+G6)/2</f>
-        <v>450</v>
+        <v>350</v>
       </c>
       <c r="H36" s="1">
         <f>(H5+H6)/2</f>
@@ -19243,7 +19243,7 @@
       </c>
       <c r="G39" s="1">
         <f t="shared" si="2"/>
-        <v>418.5</v>
+        <v>325.5</v>
       </c>
       <c r="H39" s="1">
         <f t="shared" si="2"/>
@@ -19280,7 +19280,7 @@
       </c>
       <c r="G40" s="1">
         <f t="shared" si="2"/>
-        <v>2.25</v>
+        <v>1.75</v>
       </c>
       <c r="H40" s="1">
         <f t="shared" si="2"/>
@@ -19354,7 +19354,7 @@
       </c>
       <c r="G42" s="1">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.35000000000000003</v>
       </c>
       <c r="H42" s="1">
         <f t="shared" si="2"/>
@@ -19391,7 +19391,7 @@
       </c>
       <c r="G43" s="1">
         <f t="shared" si="2"/>
-        <v>3.6</v>
+        <v>2.8000000000000003</v>
       </c>
       <c r="H43" s="1">
         <f t="shared" si="2"/>
@@ -19428,7 +19428,7 @@
       </c>
       <c r="G44" s="1">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H44" s="1">
         <f t="shared" si="2"/>
@@ -19465,7 +19465,7 @@
       </c>
       <c r="G45" s="1">
         <f t="shared" si="2"/>
-        <v>13.5</v>
+        <v>10.5</v>
       </c>
       <c r="H45" s="1">
         <f t="shared" si="2"/>
@@ -19539,7 +19539,7 @@
       </c>
       <c r="G47" s="1">
         <f t="shared" si="2"/>
-        <v>0.9</v>
+        <v>0.70000000000000007</v>
       </c>
       <c r="H47" s="1">
         <f t="shared" si="2"/>
@@ -19576,7 +19576,7 @@
       </c>
       <c r="G48" s="1">
         <f t="shared" si="2"/>
-        <v>0.9</v>
+        <v>0.70000000000000007</v>
       </c>
       <c r="H48" s="1">
         <f t="shared" si="2"/>
@@ -19613,7 +19613,7 @@
       </c>
       <c r="G49" s="1">
         <f t="shared" si="2"/>
-        <v>0.9</v>
+        <v>0.70000000000000007</v>
       </c>
       <c r="H49" s="1">
         <f t="shared" si="2"/>

</xml_diff>